<commit_message>
added create, add and display art features
</commit_message>
<xml_diff>
--- a/planning/planning.xlsx
+++ b/planning/planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aprilcanete/Desktop/GA-SEI/artzy/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3063C0A6-D9E9-B247-95DF-3401222BACD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B43AA06-5F10-B540-91B9-8C8E09EED935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48960" yWindow="3680" windowWidth="33560" windowHeight="16640" xr2:uid="{8869013C-6BD3-9241-A9E3-4A965B6B46B8}"/>
+    <workbookView xWindow="48960" yWindow="3680" windowWidth="26720" windowHeight="16640" xr2:uid="{8869013C-6BD3-9241-A9E3-4A965B6B46B8}"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="112">
   <si>
     <t>actions/requests</t>
   </si>
@@ -331,13 +331,55 @@
   </si>
   <si>
     <t>In progress</t>
+  </si>
+  <si>
+    <t>Web design</t>
+  </si>
+  <si>
+    <t>Add css styling</t>
+  </si>
+  <si>
+    <t>Register page css</t>
+  </si>
+  <si>
+    <t>login page css</t>
+  </si>
+  <si>
+    <t>logout feature css</t>
+  </si>
+  <si>
+    <t>profile page css</t>
+  </si>
+  <si>
+    <t>show page css</t>
+  </si>
+  <si>
+    <t>home page css</t>
+  </si>
+  <si>
+    <t>6.1.1</t>
+  </si>
+  <si>
+    <t>6.1.2</t>
+  </si>
+  <si>
+    <t>6.1.3</t>
+  </si>
+  <si>
+    <t>6.1.4</t>
+  </si>
+  <si>
+    <t>6.1.5</t>
+  </si>
+  <si>
+    <t>6.1.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -360,6 +402,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Avenir Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Avenir Book"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -557,7 +612,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -593,19 +648,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1428,175 +1491,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF85EC1A-2CB7-FD42-8EF3-6C7493CCABF4}">
-  <dimension ref="A2:D18"/>
+  <dimension ref="A2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="1" max="1" width="5" style="23" customWidth="1"/>
     <col min="2" max="2" width="26.5" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="25" t="s">
         <v>78</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="22" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="25" t="s">
         <v>79</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="25" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
         <v>4</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="27" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="C6" s="25"/>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="28" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
         <v>4.2</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="29" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
         <v>4.3</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="29" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="28" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="C10" s="25"/>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
         <v>4.5</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="28" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="C11" s="25"/>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="28" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="C12" s="25"/>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
         <v>4.7</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="28" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="C13" s="25"/>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
         <v>4.8</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="28" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="C14" s="25"/>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="28" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="C15" s="25"/>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A16" s="24">
         <v>5</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="27" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="C16" s="25"/>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="30" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="C17" s="25"/>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A18" s="24">
         <v>5.2</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="30" t="s">
         <v>94</v>
       </c>
+      <c r="C18" s="25"/>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>6</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="25"/>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A20" s="24">
+        <v>6.1</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="25"/>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="25"/>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="25"/>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="25"/>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="25"/>
+    </row>
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="25"/>
+    </row>
+    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>